<commit_message>
[code can now update complete data based on google form responses]
</commit_message>
<xml_diff>
--- a/Data Processing/Data Submissions (Responses).xlsx
+++ b/Data Processing/Data Submissions (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="108">
   <si>
     <t>Timestamp</t>
   </si>
@@ -100,20 +100,251 @@
     <t>Your Name</t>
   </si>
   <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>bye</t>
+    <t>Proteome of the Developing Murine Lens Through Mass Spectrometry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://iovs.arvojournals.org/article.aspx?articleid=2670138</t>
+  </si>
+  <si>
+    <t>PXD006381</t>
+  </si>
+  <si>
+    <t>Mus musculus (mouse)</t>
+  </si>
+  <si>
+    <t>Lens of camera-type eye</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>Time points: Embryonic day 15 (E15) and 18 (E18) and postnatal day 0 (P0), 3 (P3), 6 (P6), and 9 (P9)</t>
+  </si>
+  <si>
+    <t>3 biological replicates for each subgroup (timepoint)</t>
+  </si>
+  <si>
+    <t>Total: 18 (3*6 = biological replicates x nTimepoint)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>https://arvo.silverchair-cdn.com/arvo/content_public/journal/iovs/936670/iovs-58-13-55_s17.xlsx?Expires=1694527471&amp;Signature=mHlI~HEy-FgNjqxvb94lFXK~l~HNZu~3jqskFnU~EYhunLtPRQBIvMmRPoXClW6m-gQDd4hjZ2XtUuEwIsyDgOKhoRN0odhGEgeFMbA5mtIAVwYy3XZ~Xkv5NfoFbU7RWjuwOOk4JgGc3TWGBVtsAZWfIIFIYwqt65MkdOQNNxi-xffZN3-ft4710Zavg6D6YhcHe-po3WVQ1iWPMOJqHESL~cmFOPgB40qAD1PZq7WInSAKoH7n-vodUu-KfsJLHxWwrAg55fGqUc0yodOU1foOHgtZjWl15-AgZKdbAks2oONvcJbGYRV0UBal3L-IiTHEdGYTgAcx52ygO9mcLg__&amp;Key-Pair-Id=APKAIE5G5CRDK6RD3PGA</t>
+  </si>
+  <si>
+    <t>Protein Expression</t>
+  </si>
+  <si>
+    <t>Labeled</t>
+  </si>
+  <si>
+    <t>TMT</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>ProteomeDiscoverer</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>6076 x 18</t>
+  </si>
+  <si>
+    <t>https://arvo.silverchair-cdn.com/arvo/content_public/journal/iovs/936670/iovs-58-13-55_s01.xlsx?Expires=1694031584&amp;Signature=SUvzQSU~dLy4kqmfCuSnLGjQ8Zt3tkeO7ycfMXP3ZDy69blYWJ6F0vQHiuXABG95NBlkmYCAq8QwV-INWSlL5HadM2N0m4Y1oXEDT8EX4rGLUazyDQRGSiOjIA~FTBFAcv70stq5Rzch7SFdDuPuoejE5XC5pKVEVET0ZsHi5dpGySWBoXnbVDa2WgQupcW4GcvuDV7Ts1JBGq0lw28Bbkqd7Hl0Y0E5MayIi0VKVTFjctGEexOHaZ9~fykVpk3tgo3oAJs6UzRJQQZKZTp4knFd8Oe2YTvNifY4C7xuqKhvMb~vxcP8QR3myiBDDpkXwgkevItqF5yXF-fIqZpSwg__&amp;Key-Pair-Id=APKAIE5G5CRDK6RD3PGA</t>
+  </si>
+  <si>
+    <t>trypsin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proteome-centric cross-omics characterization and integrated network analyses of triple-negative breast cancer </t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S2211124722001875?via%3Dihub</t>
+  </si>
+  <si>
+    <t>IPX0003222000</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Breast tumor and non-cancerous adjacent tissue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUSCCTNBC cohort </t>
+  </si>
+  <si>
+    <t>Breast cancer and non-cancerous tissue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90 FUSCCTNBC cohort </t>
+  </si>
+  <si>
+    <t>Total: 90</t>
+  </si>
+  <si>
+    <t>https://ars.els-cdn.com/content/image/1-s2.0-S2211124722001875-mmc2.xlsx</t>
+  </si>
+  <si>
+    <t>Phosphorylation</t>
+  </si>
+  <si>
+    <t>Label free</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>MaxQuant</t>
+  </si>
+  <si>
+    <t>https://ars.els-cdn.com/content/image/1-s2.0-S2211124722001875-mmc3.xlsx</t>
+  </si>
+  <si>
+    <t>20069 x 86, 70</t>
+  </si>
+  <si>
+    <t>7531 x 82, 66</t>
+  </si>
+  <si>
+    <t>Trypsin</t>
+  </si>
+  <si>
+    <t>Identification of Salivary Biomarkers for Oral Cancer Detection with Untargeted and Targeted Quantitative Proteomics Approaches</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6731081/</t>
+  </si>
+  <si>
+    <t>PXD008655</t>
+  </si>
+  <si>
+    <t>Saliva</t>
+  </si>
+  <si>
+    <t>HC, OPMD, OSCC cohorts</t>
+  </si>
+  <si>
+    <t>healthy, potentially malignant, oral squamous cell carcinoma</t>
+  </si>
+  <si>
+    <t>115 HC, 116 OPMD, 117 OSCC</t>
+  </si>
+  <si>
+    <t>Total: 348</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6731081/bin/152475_0_supp_321761_pqpfdb.xlsx</t>
+  </si>
+  <si>
+    <t>Protein expression</t>
+  </si>
+  <si>
+    <t>iTRAQ</t>
+  </si>
+  <si>
+    <t>Proteome Discoverer</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6731081/bin/152475_0_supp_321762_pqpfdb.xlsx</t>
+  </si>
+  <si>
+    <t>45062 x 348</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>1838 x 348</t>
+  </si>
+  <si>
+    <t>Inhaled multi-walled carbon nanotubes differently modulate global gene and protein expression in rat lungs</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/full/10.1080/17435390.2020.1851418</t>
+  </si>
+  <si>
+    <t>PXD029842</t>
+  </si>
+  <si>
+    <t>Rattus norvegicus (rat)</t>
+  </si>
+  <si>
+    <t>Lung tissue</t>
+  </si>
+  <si>
+    <t>Multi-walled carbon nanotubes inhaled: NM-401, NM-403</t>
+  </si>
+  <si>
+    <t>Recovery Period (RP): 3/30/90/180 days, Dosage: High, Low</t>
+  </si>
+  <si>
+    <t>6 rats for each group</t>
+  </si>
+  <si>
+    <t>Total: 48 (6 x nRP x nDosage = 6 x 4 x 2)</t>
+  </si>
+  <si>
+    <t>Label Free</t>
+  </si>
+  <si>
+    <t>1175 x 48</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/suppl/10.1080/17435390.2020.1851418?scroll=top&amp;role=tab#:~:text=Share-,Download,-figshare -Supplementary file 8</t>
+  </si>
+  <si>
+    <t>"Mass Spectrometry-Based Proteomics Analysis of Human Substantia Nigra From Parkinson's Disease Patients Identifies Multiple Pathways Potentially Involved in the Disease "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcponline.org/article/S1535-9476(22)00260-2/fulltext </t>
+  </si>
+  <si>
+    <t>Substantia Nigra</t>
+  </si>
+  <si>
+    <t>Parkinson's vs healthy</t>
+  </si>
+  <si>
+    <t>Main and replication experiment; FDR calculation with and without permutations in groups</t>
+  </si>
+  <si>
+    <t>15 for each group</t>
+  </si>
+  <si>
+    <t>15*2 = 30 samples total</t>
+  </si>
+  <si>
+    <t>http://efaidnbmnnnibpcajpcglclefindmkaj/https://www.mcponline.org/cms/10.1016/j.mcpro.2022.100452/attachment/bd62a816-b040-43ea-b97e-410198cdacb7/mmc8.pdf</t>
+  </si>
+  <si>
+    <t>"Protein Expression "</t>
+  </si>
+  <si>
+    <t>https://www.mcponline.org/cms/10.1016/j.mcpro.2022.100280/attachment/439cf0fb-1eac-48a2-b7ae-ab88bb45fc83/mmc6.xlsx -Given in 2nd coloumn of supplementary data S1</t>
+  </si>
+  <si>
+    <t>134787 x 66</t>
+  </si>
+  <si>
+    <t>9743 x 30</t>
+  </si>
+  <si>
+    <t>Given in 1st column of supplementary data S1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -124,6 +355,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,12 +379,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -460,19 +708,418 @@
       </c>
     </row>
     <row r="2">
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2">
+        <v>45208.80736532407</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2.9332127E7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="s">
-        <v>31</v>
+      <c r="A3" s="2">
+        <v>45208.81954616898</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3.5235781E7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>45208.82131158565</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3.1253657E7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>45208.812024513885</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3.3332178E7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>45208.81447565972</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3.6423813E7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="M2"/>
+    <hyperlink r:id="rId3" ref="X2"/>
+    <hyperlink r:id="rId4" ref="C3"/>
+    <hyperlink r:id="rId5" ref="M3"/>
+    <hyperlink r:id="rId6" ref="T3"/>
+    <hyperlink r:id="rId7" ref="X3"/>
+    <hyperlink r:id="rId8" ref="C4"/>
+    <hyperlink r:id="rId9" ref="M4"/>
+    <hyperlink r:id="rId10" ref="T4"/>
+    <hyperlink r:id="rId11" ref="C5"/>
+    <hyperlink r:id="rId12" ref="C6"/>
+    <hyperlink r:id="rId13" ref="M6"/>
+  </hyperlinks>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>